<commit_message>
Updated readmes for libstdc++
</commit_message>
<xml_diff>
--- a/msvs.xlsx
+++ b/msvs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="8295" windowWidth="34350" windowHeight="16770"/>
+    <workbookView xWindow="90" yWindow="255" windowWidth="34350" windowHeight="16770" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sorted" sheetId="1" r:id="rId1"/>
@@ -934,25 +934,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="156770304"/>
-        <c:axId val="156771840"/>
+        <c:axId val="19394560"/>
+        <c:axId val="19396096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156770304"/>
+        <c:axId val="19394560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156771840"/>
+        <c:crossAx val="19396096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156771840"/>
+        <c:axId val="19396096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -979,7 +978,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156770304"/>
+        <c:crossAx val="19394560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -989,7 +988,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1031,160 +1030,160 @@
               <c:strCache>
                 <c:ptCount val="92"/>
                 <c:pt idx="0">
-                  <c:v>ranges</c:v>
+                  <c:v>climits</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>version</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>climits</c:v>
+                  <c:v>compare</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>cfloat</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>cstddef</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>initializer_list</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>cerrno</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>cstdalign</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>cstdarg</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>cassert</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>ciso646</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>clocale</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>csetjmp</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>csignal</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>cstdbool</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>cuchar</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>cinttypes</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>cstdint</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>cfenv</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>cwctype</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>cctype</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>ctime</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>cstring</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>cstdlib</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>cstdio</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>cmath</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>type_traits</c:v>
+                </c:pt>
+                <c:pt idx="27">
                   <c:v>concepts</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>compare</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>cfloat</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>cstddef</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>initializer_list</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>cassert</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>cerrno</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>csignal</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>cstdarg</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>cstdbool</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>ciso646</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>csetjmp</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>cstdalign</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>cstdint</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>cuchar</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>clocale</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>cfenv</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>cinttypes</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>cwctype</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>cctype</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>ctime</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>cstring</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>cstdlib</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>cstdio</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>cmath</c:v>
-                </c:pt>
                 <c:pt idx="28">
-                  <c:v>type_traits</c:v>
+                  <c:v>ratio</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>ratio</c:v>
+                  <c:v>utility</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>utility</c:v>
+                  <c:v>exception</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>exception</c:v>
+                  <c:v>new</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>new</c:v>
+                  <c:v>typeinfo</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>typeindex</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>typeinfo</c:v>
+                  <c:v>cwchar</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>cwchar</c:v>
+                  <c:v>atomic</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>atomic</c:v>
+                  <c:v>limits</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>tuple</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>limits</c:v>
+                  <c:v>iosfwd</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>iosfwd</c:v>
+                  <c:v>chrono</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>chrono</c:v>
+                  <c:v>charconv</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>charconv</c:v>
+                  <c:v>numeric</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>numeric</c:v>
+                  <c:v>any</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>any</c:v>
+                  <c:v>optional</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>optional</c:v>
+                  <c:v>scoped_allocator</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>scoped_allocator</c:v>
+                  <c:v>memory</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>memory</c:v>
+                  <c:v>deque</c:v>
                 </c:pt>
                 <c:pt idx="47">
+                  <c:v>list</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>stack</c:v>
+                </c:pt>
+                <c:pt idx="49">
                   <c:v>forward_list</c:v>
                 </c:pt>
-                <c:pt idx="48">
-                  <c:v>list</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>deque</c:v>
-                </c:pt>
                 <c:pt idx="50">
-                  <c:v>stack</c:v>
+                  <c:v>map</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>set</c:v>
+                  <c:v>valarray</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>vector</c:v>
@@ -1193,106 +1192,106 @@
                   <c:v>algorithm</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>map</c:v>
+                  <c:v>set</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>valarray</c:v>
+                  <c:v>stdexcept</c:v>
                 </c:pt>
                 <c:pt idx="56">
                   <c:v>thread</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>stdexcept</c:v>
+                  <c:v>string_view</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>string_view</c:v>
+                  <c:v>bitset</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>bitset</c:v>
+                  <c:v>string</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>system_error</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>string</c:v>
+                  <c:v>queue</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>queue</c:v>
+                  <c:v>variant</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>variant</c:v>
+                  <c:v>condition_variable</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>condition_variable</c:v>
+                  <c:v>mutex</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>mutex</c:v>
+                  <c:v>shared_mutex</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>shared_mutex</c:v>
+                  <c:v>unordered_set</c:v>
                 </c:pt>
                 <c:pt idx="67">
                   <c:v>streambuf</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>unordered_set</c:v>
+                  <c:v>unordered_map</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>unordered_map</c:v>
+                  <c:v>memory_resource</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>memory_resource</c:v>
+                  <c:v>ios</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>ios</c:v>
+                  <c:v>random</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>functional</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>random</c:v>
+                  <c:v>ostream</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>ostream</c:v>
+                  <c:v>istream</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>istream</c:v>
+                  <c:v>iostream</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>iostream</c:v>
+                  <c:v>locale</c:v>
                 </c:pt>
                 <c:pt idx="77">
+                  <c:v>codecvt</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>strstream</c:v>
+                </c:pt>
+                <c:pt idx="79">
                   <c:v>iterator</c:v>
                 </c:pt>
-                <c:pt idx="78">
-                  <c:v>locale</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>strstream</c:v>
-                </c:pt>
                 <c:pt idx="80">
-                  <c:v>codecvt</c:v>
+                  <c:v>sstream</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>sstream</c:v>
+                  <c:v>ranges</c:v>
                 </c:pt>
                 <c:pt idx="82">
+                  <c:v>complex</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>ccomplex</c:v>
+                </c:pt>
+                <c:pt idx="84">
                   <c:v>fstream</c:v>
                 </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="85">
+                  <c:v>ctgmath</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>array</c:v>
+                </c:pt>
+                <c:pt idx="87">
                   <c:v>iomanip</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>complex</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>ccomplex</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>ctgmath</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>array</c:v>
                 </c:pt>
                 <c:pt idx="88">
                   <c:v>execution</c:v>
@@ -1316,43 +1315,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="92"/>
                 <c:pt idx="0">
-                  <c:v>0.34375</c:v>
+                  <c:v>0.359375</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34375</c:v>
+                  <c:v>0.359375</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.359375</c:v>
+                  <c:v>0.390625</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.375</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.390625</c:v>
+                  <c:v>0.515625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.53125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>0.5625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5</c:v>
+                  <c:v>0.5625</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.5625</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.578125</c:v>
@@ -1364,255 +1363,255 @@
                   <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.578125</c:v>
+                  <c:v>0.59375</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.578125</c:v>
+                  <c:v>0.59375</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.59375</c:v>
+                  <c:v>0.609375</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.609375</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.609375</c:v>
+                  <c:v>0.65625</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.609375</c:v>
+                  <c:v>0.671875</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.65625</c:v>
+                  <c:v>0.90625</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.671875</c:v>
+                  <c:v>1.140625</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.90625</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.125</c:v>
+                  <c:v>1.421875</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.234375</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.421875</c:v>
+                  <c:v>1.515625</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.46875</c:v>
+                  <c:v>1.546875</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.5</c:v>
+                  <c:v>1.5625</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.515625</c:v>
+                  <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.625</c:v>
+                  <c:v>1.65625</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.640625</c:v>
+                  <c:v>1.65625</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.640625</c:v>
+                  <c:v>1.671875</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.640625</c:v>
+                  <c:v>1.828125</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.8125</c:v>
+                  <c:v>2.09375</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.078125</c:v>
+                  <c:v>2.53125</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.453125</c:v>
+                  <c:v>2.578125</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.515625</c:v>
+                  <c:v>2.71875</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.6875</c:v>
+                  <c:v>3.15625</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.109375</c:v>
+                  <c:v>3.390625</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.296875</c:v>
+                  <c:v>3.640625</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.53125</c:v>
+                  <c:v>3.828125</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.71875</c:v>
+                  <c:v>3.859375</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.765625</c:v>
+                  <c:v>3.984375</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.84375</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.890625</c:v>
+                  <c:v>4.03125</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.921875</c:v>
+                  <c:v>4.046875</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.921875</c:v>
+                  <c:v>4.046875</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.9375</c:v>
+                  <c:v>4.0625</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.96875</c:v>
+                  <c:v>4.140625</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.015625</c:v>
+                  <c:v>4.140625</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.015625</c:v>
+                  <c:v>4.140625</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.03125</c:v>
+                  <c:v>4.203125</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.03125</c:v>
+                  <c:v>4.203125</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.03125</c:v>
+                  <c:v>4.40625</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.25</c:v>
+                  <c:v>4.40625</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.28125</c:v>
+                  <c:v>4.421875</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.296875</c:v>
+                  <c:v>4.4375</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.3125</c:v>
+                  <c:v>4.46875</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4.328125</c:v>
+                  <c:v>4.46875</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.375</c:v>
+                  <c:v>4.671875</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4.609375</c:v>
+                  <c:v>4.921875</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4.765625</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.875</c:v>
+                  <c:v>5.078125</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.890625</c:v>
+                  <c:v>5.09375</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.921875</c:v>
+                  <c:v>5.125</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5</c:v>
+                  <c:v>5.171875</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.03125</c:v>
+                  <c:v>5.265625</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.078125</c:v>
+                  <c:v>5.3125</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.15625</c:v>
+                  <c:v>5.546875</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.375</c:v>
+                  <c:v>5.609375</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>5.40625</c:v>
+                  <c:v>5.640625</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>5.46875</c:v>
+                  <c:v>5.65625</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>5.484375</c:v>
+                  <c:v>5.734375</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>5.609375</c:v>
+                  <c:v>5.765625</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>5.671875</c:v>
+                  <c:v>5.796875</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>5.671875</c:v>
+                  <c:v>5.828125</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>5.671875</c:v>
+                  <c:v>5.828125</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>5.671875</c:v>
+                  <c:v>5.84375</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>5.703125</c:v>
+                  <c:v>5.84375</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>5.71875</c:v>
+                  <c:v>5.875</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>5.765625</c:v>
+                  <c:v>5.96875</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>5.875</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>5.890625</c:v>
+                  <c:v>6.015625</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>5.90625</c:v>
+                  <c:v>6.078125</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>5.90625</c:v>
+                  <c:v>6.125</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>6</c:v>
+                  <c:v>6.140625</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>6.265625</c:v>
+                  <c:v>6.390625</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>6.890625</c:v>
+                  <c:v>7.0625</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>7.109375</c:v>
+                  <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>7.90625</c:v>
+                  <c:v>8.171875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="182753920"/>
-        <c:axId val="182223232"/>
+        <c:axId val="46841216"/>
+        <c:axId val="46864640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="182753920"/>
+        <c:axId val="46841216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182223232"/>
+        <c:crossAx val="46864640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="182223232"/>
+        <c:axId val="46864640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -1639,7 +1638,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="182753920"/>
+        <c:crossAx val="46841216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1649,7 +1648,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1670,7 +1669,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Mean increase VS2017 -&gt; VS2019 is -12%</a:t>
+              <a:t>Median decrease VS2017 -&gt; VS2019 is 9%</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2566,25 +2565,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="92"/>
                 <c:pt idx="0">
-                  <c:v>4.03125</c:v>
+                  <c:v>4.203125</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.71875</c:v>
+                  <c:v>3.828125</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>6.125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.09375</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.578125</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.078125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.3125</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.5625</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>5.90625</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.65625</c:v>
@@ -2599,13 +2598,13 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.296875</c:v>
+                  <c:v>3.390625</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.109375</c:v>
+                  <c:v>3.15625</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.609375</c:v>
+                  <c:v>0.59375</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.578125</c:v>
@@ -2614,58 +2613,58 @@
                   <c:v>0.359375</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.59375</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1.421875</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.703125</c:v>
+                  <c:v>5.828125</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0.390625</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.890625</c:v>
+                  <c:v>5.96875</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.375</c:v>
+                  <c:v>1.515625</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.875</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="24">
+                  <c:v>0.578125</c:v>
+                </c:pt>
+                <c:pt idx="25">
                   <c:v>0.5625</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>0.5625</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.5625</c:v>
+                  <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.5</c:v>
+                  <c:v>0.515625</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.578125</c:v>
+                  <c:v>0.59375</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.234375</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.125</c:v>
+                  <c:v>1.140625</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>0.90625</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.90625</c:v>
+                  <c:v>6.078125</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>0.671875</c:v>
@@ -2674,197 +2673,196 @@
                   <c:v>0.578125</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.8125</c:v>
+                  <c:v>1.828125</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>0.609375</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.9375</c:v>
+                  <c:v>4.03125</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.265625</c:v>
+                  <c:v>6.390625</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7.109375</c:v>
+                  <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.921875</c:v>
+                  <c:v>4.0625</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>6.015625</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.640625</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>8.171875</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.53125</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.140625</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.546875</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.71875</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>5.765625</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.40625</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>7.90625</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="51">
+                  <c:v>5.734375</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.84375</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.53125</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.046875</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.796875</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.140625</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.3125</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.078125</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.65625</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.640625</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.859375</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.65625</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.671875</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.609375</c:v>
+                </c:pt>
+                <c:pt idx="66">
                   <c:v>5.875</c:v>
                 </c:pt>
-                <c:pt idx="48">
-                  <c:v>5.375</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>2.6875</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>5.671875</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5.609375</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5.671875</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2.515625</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3.921875</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5.671875</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>4.03125</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3.890625</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.15625</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>4.890625</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1.640625</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>3.53125</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3.765625</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5.484375</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>4.609375</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5.46875</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.34375</c:v>
-                </c:pt>
                 <c:pt idx="67">
+                  <c:v>1.546875</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7.0625</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.984375</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4.203125</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5.09375</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>5.84375</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4.046875</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4.40625</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5.171875</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>4.46875</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>4.421875</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5.828125</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>4.46875</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4.40625</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2.578125</c:v>
+                </c:pt>
+                <c:pt idx="82">
                   <c:v>1.5</c:v>
                 </c:pt>
-                <c:pt idx="68">
-                  <c:v>6.890625</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>3.84375</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>4.015625</c:v>
-                </c:pt>
-                <c:pt idx="71">
+                <c:pt idx="83">
+                  <c:v>1.671875</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.65625</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5.265625</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5.125</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.5625</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>4.140625</c:v>
+                </c:pt>
+                <c:pt idx="89">
                   <c:v>4.921875</c:v>
                 </c:pt>
-                <c:pt idx="72">
-                  <c:v>5.71875</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>3.96875</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>4.28125</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>4.375</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>4.296875</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>5.671875</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>4.328125</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>2.453125</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>1.46875</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>1.640625</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>1.640625</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>5.078125</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>5.03125</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>1.515625</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>4.03125</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>4.765625</c:v>
-                </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.015625</c:v>
+                  <c:v>4.140625</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.34375</c:v>
+                  <c:v>0.359375</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="156905856"/>
-        <c:axId val="156907392"/>
+        <c:axId val="48233088"/>
+        <c:axId val="149577088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="156905856"/>
+        <c:axId val="48233088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156907392"/>
+        <c:crossAx val="149577088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="156907392"/>
+        <c:axId val="149577088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -2891,7 +2889,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="156905856"/>
+        <c:crossAx val="48233088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2905,7 +2903,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3302,8 +3300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3338,10 +3336,10 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>0.34375</v>
+        <v>0.359375</v>
       </c>
       <c r="E3" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3352,7 +3350,7 @@
         <v>74</v>
       </c>
       <c r="D4">
-        <v>0.34375</v>
+        <v>0.359375</v>
       </c>
       <c r="E4" t="s">
         <v>91</v>
@@ -3366,10 +3364,10 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0.359375</v>
+        <v>0.390625</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -3380,10 +3378,10 @@
         <v>4</v>
       </c>
       <c r="D6">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="E6" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -3394,10 +3392,10 @@
         <v>8</v>
       </c>
       <c r="D7">
-        <v>0.390625</v>
+        <v>0.515625</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -3408,10 +3406,10 @@
         <v>85</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0.53125</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -3422,10 +3420,10 @@
         <v>11</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0.5625</v>
       </c>
       <c r="E9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -3436,10 +3434,10 @@
         <v>86</v>
       </c>
       <c r="D10">
-        <v>0.5</v>
+        <v>0.5625</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -3453,7 +3451,7 @@
         <v>0.5625</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -3464,10 +3462,10 @@
         <v>87</v>
       </c>
       <c r="D12">
-        <v>0.5625</v>
+        <v>0.578125</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -3478,10 +3476,10 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>0.5625</v>
+        <v>0.578125</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -3492,10 +3490,10 @@
         <v>56</v>
       </c>
       <c r="D14">
-        <v>0.5625</v>
+        <v>0.578125</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -3506,10 +3504,10 @@
         <v>76</v>
       </c>
       <c r="D15">
-        <v>0.5625</v>
+        <v>0.578125</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -3523,7 +3521,7 @@
         <v>0.578125</v>
       </c>
       <c r="E16" t="s">
-        <v>87</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -3537,7 +3535,7 @@
         <v>0.578125</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -3551,7 +3549,7 @@
         <v>0.578125</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -3562,10 +3560,10 @@
         <v>73</v>
       </c>
       <c r="D19">
-        <v>0.578125</v>
+        <v>0.59375</v>
       </c>
       <c r="E19" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -3576,10 +3574,10 @@
         <v>19</v>
       </c>
       <c r="D20">
-        <v>0.578125</v>
+        <v>0.59375</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -3590,10 +3588,10 @@
         <v>7</v>
       </c>
       <c r="D21">
-        <v>0.59375</v>
+        <v>0.609375</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -3607,7 +3605,7 @@
         <v>0.609375</v>
       </c>
       <c r="E22" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -3618,10 +3616,10 @@
         <v>15</v>
       </c>
       <c r="D23">
-        <v>0.609375</v>
+        <v>0.65625</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3632,10 +3630,10 @@
         <v>18</v>
       </c>
       <c r="D24">
-        <v>0.609375</v>
+        <v>0.671875</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -3646,10 +3644,10 @@
         <v>17</v>
       </c>
       <c r="D25">
-        <v>0.65625</v>
+        <v>0.90625</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -3660,10 +3658,10 @@
         <v>13</v>
       </c>
       <c r="D26">
-        <v>0.671875</v>
+        <v>1.140625</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -3674,10 +3672,10 @@
         <v>24</v>
       </c>
       <c r="D27">
-        <v>0.90625</v>
+        <v>1.25</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -3688,10 +3686,10 @@
         <v>22</v>
       </c>
       <c r="D28">
-        <v>1.125</v>
+        <v>1.421875</v>
       </c>
       <c r="E28" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -3702,10 +3700,10 @@
         <v>58</v>
       </c>
       <c r="D29">
-        <v>1.234375</v>
+        <v>1.5</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -3716,10 +3714,10 @@
         <v>20</v>
       </c>
       <c r="D30">
-        <v>1.421875</v>
+        <v>1.515625</v>
       </c>
       <c r="E30" t="s">
-        <v>13</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -3730,10 +3728,10 @@
         <v>14</v>
       </c>
       <c r="D31">
-        <v>1.46875</v>
+        <v>1.546875</v>
       </c>
       <c r="E31" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -3744,10 +3742,10 @@
         <v>16</v>
       </c>
       <c r="D32">
-        <v>1.5</v>
+        <v>1.5625</v>
       </c>
       <c r="E32" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -3758,10 +3756,10 @@
         <v>57</v>
       </c>
       <c r="D33">
-        <v>1.515625</v>
+        <v>1.625</v>
       </c>
       <c r="E33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -3772,10 +3770,10 @@
         <v>23</v>
       </c>
       <c r="D34">
-        <v>1.625</v>
+        <v>1.65625</v>
       </c>
       <c r="E34" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -3786,10 +3784,10 @@
         <v>25</v>
       </c>
       <c r="D35">
-        <v>1.640625</v>
+        <v>1.65625</v>
       </c>
       <c r="E35" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -3800,7 +3798,7 @@
         <v>21</v>
       </c>
       <c r="D36">
-        <v>1.640625</v>
+        <v>1.671875</v>
       </c>
       <c r="E36" t="s">
         <v>57</v>
@@ -3814,10 +3812,10 @@
         <v>50</v>
       </c>
       <c r="D37">
-        <v>1.640625</v>
+        <v>1.828125</v>
       </c>
       <c r="E37" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -3828,10 +3826,10 @@
         <v>60</v>
       </c>
       <c r="D38">
-        <v>1.8125</v>
+        <v>2.09375</v>
       </c>
       <c r="E38" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -3842,10 +3840,10 @@
         <v>59</v>
       </c>
       <c r="D39">
-        <v>2.078125</v>
+        <v>2.53125</v>
       </c>
       <c r="E39" t="s">
-        <v>69</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3856,7 +3854,7 @@
         <v>77</v>
       </c>
       <c r="D40">
-        <v>2.453125</v>
+        <v>2.578125</v>
       </c>
       <c r="E40" t="s">
         <v>60</v>
@@ -3870,10 +3868,10 @@
         <v>78</v>
       </c>
       <c r="D41">
-        <v>2.515625</v>
+        <v>2.71875</v>
       </c>
       <c r="E41" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3884,10 +3882,10 @@
         <v>81</v>
       </c>
       <c r="D42">
-        <v>2.6875</v>
+        <v>3.15625</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -3898,10 +3896,10 @@
         <v>63</v>
       </c>
       <c r="D43">
-        <v>3.109375</v>
+        <v>3.390625</v>
       </c>
       <c r="E43" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3912,10 +3910,10 @@
         <v>28</v>
       </c>
       <c r="D44">
-        <v>3.296875</v>
+        <v>3.640625</v>
       </c>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3926,10 +3924,10 @@
         <v>27</v>
       </c>
       <c r="D45">
-        <v>3.53125</v>
+        <v>3.828125</v>
       </c>
       <c r="E45" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3940,10 +3938,10 @@
         <v>36</v>
       </c>
       <c r="D46">
-        <v>3.71875</v>
+        <v>3.859375</v>
       </c>
       <c r="E46" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3954,10 +3952,10 @@
         <v>40</v>
       </c>
       <c r="D47">
-        <v>3.765625</v>
+        <v>3.984375</v>
       </c>
       <c r="E47" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -3968,10 +3966,10 @@
         <v>61</v>
       </c>
       <c r="D48">
-        <v>3.84375</v>
+        <v>4</v>
       </c>
       <c r="E48" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3982,10 +3980,10 @@
         <v>62</v>
       </c>
       <c r="D49">
-        <v>3.890625</v>
+        <v>4.03125</v>
       </c>
       <c r="E49" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -3996,10 +3994,10 @@
         <v>52</v>
       </c>
       <c r="D50">
-        <v>3.921875</v>
+        <v>4.046875</v>
       </c>
       <c r="E50" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -4010,10 +4008,10 @@
         <v>38</v>
       </c>
       <c r="D51">
-        <v>3.921875</v>
+        <v>4.046875</v>
       </c>
       <c r="E51" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -4024,10 +4022,10 @@
         <v>43</v>
       </c>
       <c r="D52">
-        <v>3.9375</v>
+        <v>4.0625</v>
       </c>
       <c r="E52" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -4038,10 +4036,10 @@
         <v>53</v>
       </c>
       <c r="D53">
-        <v>3.96875</v>
+        <v>4.140625</v>
       </c>
       <c r="E53" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -4052,10 +4050,10 @@
         <v>48</v>
       </c>
       <c r="D54">
-        <v>4.015625</v>
+        <v>4.140625</v>
       </c>
       <c r="E54" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -4066,7 +4064,7 @@
         <v>26</v>
       </c>
       <c r="D55">
-        <v>4.015625</v>
+        <v>4.140625</v>
       </c>
       <c r="E55" t="s">
         <v>43</v>
@@ -4080,7 +4078,7 @@
         <v>49</v>
       </c>
       <c r="D56">
-        <v>4.03125</v>
+        <v>4.203125</v>
       </c>
       <c r="E56" t="s">
         <v>36</v>
@@ -4094,10 +4092,10 @@
         <v>51</v>
       </c>
       <c r="D57">
-        <v>4.03125</v>
+        <v>4.203125</v>
       </c>
       <c r="E57" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -4108,10 +4106,10 @@
         <v>35</v>
       </c>
       <c r="D58">
-        <v>4.03125</v>
+        <v>4.40625</v>
       </c>
       <c r="E58" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -4122,7 +4120,7 @@
         <v>44</v>
       </c>
       <c r="D59">
-        <v>4.25</v>
+        <v>4.40625</v>
       </c>
       <c r="E59" t="s">
         <v>68</v>
@@ -4136,10 +4134,10 @@
         <v>54</v>
       </c>
       <c r="D60">
-        <v>4.28125</v>
+        <v>4.421875</v>
       </c>
       <c r="E60" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -4150,10 +4148,10 @@
         <v>79</v>
       </c>
       <c r="D61">
-        <v>4.296875</v>
+        <v>4.4375</v>
       </c>
       <c r="E61" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -4164,10 +4162,10 @@
         <v>32</v>
       </c>
       <c r="D62">
-        <v>4.3125</v>
+        <v>4.46875</v>
       </c>
       <c r="E62" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -4178,7 +4176,7 @@
         <v>69</v>
       </c>
       <c r="D63">
-        <v>4.328125</v>
+        <v>4.46875</v>
       </c>
       <c r="E63" t="s">
         <v>61</v>
@@ -4192,10 +4190,10 @@
         <v>55</v>
       </c>
       <c r="D64">
-        <v>4.375</v>
+        <v>4.671875</v>
       </c>
       <c r="E64" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -4206,10 +4204,10 @@
         <v>45</v>
       </c>
       <c r="D65">
-        <v>4.609375</v>
+        <v>4.921875</v>
       </c>
       <c r="E65" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -4220,10 +4218,10 @@
         <v>29</v>
       </c>
       <c r="D66">
-        <v>4.765625</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -4234,10 +4232,10 @@
         <v>34</v>
       </c>
       <c r="D67">
-        <v>4.875</v>
+        <v>5.078125</v>
       </c>
       <c r="E67" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -4248,10 +4246,10 @@
         <v>47</v>
       </c>
       <c r="D68">
-        <v>4.890625</v>
+        <v>5.09375</v>
       </c>
       <c r="E68" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -4262,10 +4260,10 @@
         <v>68</v>
       </c>
       <c r="D69">
-        <v>4.921875</v>
+        <v>5.125</v>
       </c>
       <c r="E69" t="s">
-        <v>82</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -4276,7 +4274,7 @@
         <v>39</v>
       </c>
       <c r="D70">
-        <v>5</v>
+        <v>5.171875</v>
       </c>
       <c r="E70" t="s">
         <v>35</v>
@@ -4290,10 +4288,10 @@
         <v>46</v>
       </c>
       <c r="D71">
-        <v>5.03125</v>
+        <v>5.265625</v>
       </c>
       <c r="E71" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -4304,10 +4302,10 @@
         <v>66</v>
       </c>
       <c r="D72">
-        <v>5.078125</v>
+        <v>5.3125</v>
       </c>
       <c r="E72" t="s">
-        <v>51</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -4318,10 +4316,10 @@
         <v>70</v>
       </c>
       <c r="D73">
-        <v>5.15625</v>
+        <v>5.546875</v>
       </c>
       <c r="E73" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -4332,10 +4330,10 @@
         <v>31</v>
       </c>
       <c r="D74">
-        <v>5.375</v>
+        <v>5.609375</v>
       </c>
       <c r="E74" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4346,7 +4344,7 @@
         <v>30</v>
       </c>
       <c r="D75">
-        <v>5.40625</v>
+        <v>5.640625</v>
       </c>
       <c r="E75" t="s">
         <v>55</v>
@@ -4360,10 +4358,10 @@
         <v>80</v>
       </c>
       <c r="D76">
-        <v>5.46875</v>
+        <v>5.65625</v>
       </c>
       <c r="E76" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -4374,10 +4372,10 @@
         <v>82</v>
       </c>
       <c r="D77">
-        <v>5.484375</v>
+        <v>5.734375</v>
       </c>
       <c r="E77" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -4388,10 +4386,10 @@
         <v>42</v>
       </c>
       <c r="D78">
-        <v>5.609375</v>
+        <v>5.765625</v>
       </c>
       <c r="E78" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -4402,10 +4400,10 @@
         <v>33</v>
       </c>
       <c r="D79">
-        <v>5.671875</v>
+        <v>5.796875</v>
       </c>
       <c r="E79" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -4416,10 +4414,10 @@
         <v>88</v>
       </c>
       <c r="D80">
-        <v>5.671875</v>
+        <v>5.828125</v>
       </c>
       <c r="E80" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -4430,10 +4428,10 @@
         <v>89</v>
       </c>
       <c r="D81">
-        <v>5.671875</v>
+        <v>5.828125</v>
       </c>
       <c r="E81" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -4444,10 +4442,10 @@
         <v>41</v>
       </c>
       <c r="D82">
-        <v>5.671875</v>
+        <v>5.84375</v>
       </c>
       <c r="E82" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -4458,10 +4456,10 @@
         <v>37</v>
       </c>
       <c r="D83">
-        <v>5.703125</v>
+        <v>5.84375</v>
       </c>
       <c r="E83" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -4472,10 +4470,10 @@
         <v>65</v>
       </c>
       <c r="D84">
-        <v>5.71875</v>
+        <v>5.875</v>
       </c>
       <c r="E84" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -4486,10 +4484,10 @@
         <v>64</v>
       </c>
       <c r="D85">
-        <v>5.765625</v>
+        <v>5.96875</v>
       </c>
       <c r="E85" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -4500,10 +4498,10 @@
         <v>67</v>
       </c>
       <c r="D86">
-        <v>5.875</v>
+        <v>6</v>
       </c>
       <c r="E86" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -4514,10 +4512,10 @@
         <v>75</v>
       </c>
       <c r="D87">
-        <v>5.890625</v>
+        <v>6.015625</v>
       </c>
       <c r="E87" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -4528,10 +4526,10 @@
         <v>83</v>
       </c>
       <c r="D88">
-        <v>5.90625</v>
+        <v>6.078125</v>
       </c>
       <c r="E88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -4542,23 +4540,23 @@
         <v>71</v>
       </c>
       <c r="D89">
-        <v>5.90625</v>
+        <v>6.125</v>
       </c>
       <c r="E89" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="D90">
-        <v>6</v>
+        <v>6.140625</v>
       </c>
       <c r="E90" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="D91">
-        <v>6.265625</v>
+        <v>6.390625</v>
       </c>
       <c r="E91" t="s">
         <v>83</v>
@@ -4566,7 +4564,7 @@
     </row>
     <row r="92" spans="1:5">
       <c r="D92">
-        <v>6.890625</v>
+        <v>7.0625</v>
       </c>
       <c r="E92" t="s">
         <v>67</v>
@@ -4574,7 +4572,7 @@
     </row>
     <row r="93" spans="1:5">
       <c r="D93">
-        <v>7.109375</v>
+        <v>7.25</v>
       </c>
       <c r="E93" t="s">
         <v>75</v>
@@ -4582,7 +4580,7 @@
     </row>
     <row r="94" spans="1:5">
       <c r="D94">
-        <v>7.90625</v>
+        <v>8.171875</v>
       </c>
       <c r="E94" t="s">
         <v>71</v>
@@ -4598,8 +4596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4615,19 +4613,19 @@
       </c>
       <c r="D1">
         <f>AVERAGE(D3:D99)</f>
-        <v>3.2195991847826089</v>
+        <v>3.3763586956521738</v>
       </c>
       <c r="E1">
         <f>MEDIAN(D3:D99)</f>
-        <v>3.8671875</v>
+        <v>4.015625</v>
       </c>
       <c r="M1" s="1">
         <f>(D1-A1)/A1</f>
-        <v>-0.12063532518053731</v>
+        <v>-7.7819816668728337E-2</v>
       </c>
       <c r="N1" s="1">
         <f>(E1-B1)/B1</f>
-        <v>-0.11921708185053381</v>
+        <v>-8.5409252669039148E-2</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -4660,7 +4658,7 @@
         <v>36</v>
       </c>
       <c r="D4">
-        <v>4.03125</v>
+        <v>4.203125</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
@@ -4674,7 +4672,7 @@
         <v>78</v>
       </c>
       <c r="D5">
-        <v>3.71875</v>
+        <v>3.828125</v>
       </c>
       <c r="E5" t="s">
         <v>78</v>
@@ -4688,7 +4686,7 @@
         <v>37</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>6.125</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
@@ -4702,7 +4700,7 @@
         <v>69</v>
       </c>
       <c r="D7">
-        <v>2.078125</v>
+        <v>2.09375</v>
       </c>
       <c r="E7" t="s">
         <v>69</v>
@@ -4716,7 +4714,7 @@
         <v>31</v>
       </c>
       <c r="D8">
-        <v>4.3125</v>
+        <v>4.4375</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
@@ -4730,7 +4728,7 @@
         <v>2</v>
       </c>
       <c r="D9">
-        <v>0.5625</v>
+        <v>0.578125</v>
       </c>
       <c r="E9" t="s">
         <v>2</v>
@@ -4744,7 +4742,7 @@
         <v>89</v>
       </c>
       <c r="D10">
-        <v>5.90625</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
         <v>89</v>
@@ -4808,7 +4806,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="D15">
-        <v>3.296875</v>
+        <v>3.390625</v>
       </c>
       <c r="E15" t="s">
         <v>94</v>
@@ -4822,7 +4820,7 @@
         <v>59</v>
       </c>
       <c r="D16">
-        <v>3.109375</v>
+        <v>3.15625</v>
       </c>
       <c r="E16" t="s">
         <v>59</v>
@@ -4836,7 +4834,7 @@
         <v>73</v>
       </c>
       <c r="D17">
-        <v>0.609375</v>
+        <v>0.59375</v>
       </c>
       <c r="E17" t="s">
         <v>73</v>
@@ -4878,7 +4876,7 @@
         <v>5</v>
       </c>
       <c r="D20">
-        <v>0.59375</v>
+        <v>0.578125</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -4906,7 +4904,7 @@
         <v>65</v>
       </c>
       <c r="D22">
-        <v>5.703125</v>
+        <v>5.828125</v>
       </c>
       <c r="E22" t="s">
         <v>65</v>
@@ -4928,7 +4926,7 @@
         <v>33</v>
       </c>
       <c r="D24">
-        <v>5.890625</v>
+        <v>5.96875</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -4936,7 +4934,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="D25">
-        <v>0.375</v>
+        <v>1.515625</v>
       </c>
       <c r="E25" t="s">
         <v>92</v>
@@ -4950,7 +4948,7 @@
         <v>70</v>
       </c>
       <c r="D26">
-        <v>4.875</v>
+        <v>5</v>
       </c>
       <c r="E26" t="s">
         <v>70</v>
@@ -4978,7 +4976,7 @@
         <v>8</v>
       </c>
       <c r="D28">
-        <v>0.5625</v>
+        <v>0.578125</v>
       </c>
       <c r="E28" t="s">
         <v>8</v>
@@ -4992,7 +4990,7 @@
         <v>85</v>
       </c>
       <c r="D29">
-        <v>0.578125</v>
+        <v>0.5625</v>
       </c>
       <c r="E29" t="s">
         <v>85</v>
@@ -5020,7 +5018,7 @@
         <v>86</v>
       </c>
       <c r="D31">
-        <v>0.5625</v>
+        <v>0.578125</v>
       </c>
       <c r="E31" t="s">
         <v>86</v>
@@ -5034,7 +5032,7 @@
         <v>6</v>
       </c>
       <c r="D32">
-        <v>0.5</v>
+        <v>0.515625</v>
       </c>
       <c r="E32" t="s">
         <v>6</v>
@@ -5048,7 +5046,7 @@
         <v>56</v>
       </c>
       <c r="D33">
-        <v>0.578125</v>
+        <v>0.59375</v>
       </c>
       <c r="E33" t="s">
         <v>56</v>
@@ -5062,7 +5060,7 @@
         <v>17</v>
       </c>
       <c r="D34">
-        <v>1.234375</v>
+        <v>1.25</v>
       </c>
       <c r="E34" t="s">
         <v>17</v>
@@ -5076,7 +5074,7 @@
         <v>18</v>
       </c>
       <c r="D35">
-        <v>1.125</v>
+        <v>1.140625</v>
       </c>
       <c r="E35" t="s">
         <v>18</v>
@@ -5104,7 +5102,7 @@
         <v>88</v>
       </c>
       <c r="D37">
-        <v>5.90625</v>
+        <v>6.078125</v>
       </c>
       <c r="E37" t="s">
         <v>88</v>
@@ -5146,7 +5144,7 @@
         <v>22</v>
       </c>
       <c r="D40">
-        <v>1.8125</v>
+        <v>1.828125</v>
       </c>
       <c r="E40" t="s">
         <v>22</v>
@@ -5174,7 +5172,7 @@
         <v>38</v>
       </c>
       <c r="D42">
-        <v>3.9375</v>
+        <v>4.03125</v>
       </c>
       <c r="E42" t="s">
         <v>38</v>
@@ -5202,7 +5200,7 @@
         <v>83</v>
       </c>
       <c r="D44">
-        <v>6.265625</v>
+        <v>6.390625</v>
       </c>
       <c r="E44" t="s">
         <v>83</v>
@@ -5216,7 +5214,7 @@
         <v>75</v>
       </c>
       <c r="D45">
-        <v>7.109375</v>
+        <v>7.25</v>
       </c>
       <c r="E45" t="s">
         <v>75</v>
@@ -5230,7 +5228,7 @@
         <v>62</v>
       </c>
       <c r="D46">
-        <v>3.921875</v>
+        <v>4.0625</v>
       </c>
       <c r="E46" t="s">
         <v>62</v>
@@ -5244,7 +5242,7 @@
         <v>39</v>
       </c>
       <c r="D47">
-        <v>5.765625</v>
+        <v>6.015625</v>
       </c>
       <c r="E47" t="s">
         <v>39</v>
@@ -5258,7 +5256,7 @@
         <v>55</v>
       </c>
       <c r="D48">
-        <v>5.40625</v>
+        <v>5.640625</v>
       </c>
       <c r="E48" t="s">
         <v>55</v>
@@ -5272,7 +5270,7 @@
         <v>71</v>
       </c>
       <c r="D49">
-        <v>7.90625</v>
+        <v>8.171875</v>
       </c>
       <c r="E49" t="s">
         <v>71</v>
@@ -5286,7 +5284,7 @@
         <v>74</v>
       </c>
       <c r="D50">
-        <v>0.5</v>
+        <v>0.53125</v>
       </c>
       <c r="E50" t="s">
         <v>74</v>
@@ -5300,7 +5298,7 @@
         <v>42</v>
       </c>
       <c r="D51">
-        <v>5.875</v>
+        <v>6.140625</v>
       </c>
       <c r="E51" t="s">
         <v>42</v>
@@ -5314,7 +5312,7 @@
         <v>44</v>
       </c>
       <c r="D52">
-        <v>5.375</v>
+        <v>5.546875</v>
       </c>
       <c r="E52" t="s">
         <v>44</v>
@@ -5328,7 +5326,7 @@
         <v>25</v>
       </c>
       <c r="D53">
-        <v>2.6875</v>
+        <v>2.71875</v>
       </c>
       <c r="E53" t="s">
         <v>25</v>
@@ -5342,7 +5340,7 @@
         <v>45</v>
       </c>
       <c r="D54">
-        <v>5.671875</v>
+        <v>5.765625</v>
       </c>
       <c r="E54" t="s">
         <v>45</v>
@@ -5356,7 +5354,7 @@
         <v>29</v>
       </c>
       <c r="D55">
-        <v>5.609375</v>
+        <v>5.734375</v>
       </c>
       <c r="E55" t="s">
         <v>29</v>
@@ -5370,7 +5368,7 @@
         <v>34</v>
       </c>
       <c r="D56">
-        <v>5.671875</v>
+        <v>5.84375</v>
       </c>
       <c r="E56" t="s">
         <v>34</v>
@@ -5384,7 +5382,7 @@
         <v>23</v>
       </c>
       <c r="D57">
-        <v>2.515625</v>
+        <v>2.53125</v>
       </c>
       <c r="E57" t="s">
         <v>23</v>
@@ -5398,7 +5396,7 @@
         <v>52</v>
       </c>
       <c r="D58">
-        <v>3.921875</v>
+        <v>4.046875</v>
       </c>
       <c r="E58" t="s">
         <v>52</v>
@@ -5412,7 +5410,7 @@
         <v>41</v>
       </c>
       <c r="D59">
-        <v>5.671875</v>
+        <v>5.796875</v>
       </c>
       <c r="E59" t="s">
         <v>41</v>
@@ -5426,7 +5424,7 @@
         <v>53</v>
       </c>
       <c r="D60">
-        <v>4.03125</v>
+        <v>4.140625</v>
       </c>
       <c r="E60" t="s">
         <v>53</v>
@@ -5440,7 +5438,7 @@
         <v>27</v>
       </c>
       <c r="D61">
-        <v>3.890625</v>
+        <v>4</v>
       </c>
       <c r="E61" t="s">
         <v>27</v>
@@ -5454,7 +5452,7 @@
         <v>80</v>
       </c>
       <c r="D62">
-        <v>5.15625</v>
+        <v>5.3125</v>
       </c>
       <c r="E62" t="s">
         <v>80</v>
@@ -5468,7 +5466,7 @@
         <v>66</v>
       </c>
       <c r="D63">
-        <v>4.890625</v>
+        <v>5.078125</v>
       </c>
       <c r="E63" t="s">
         <v>66</v>
@@ -5482,7 +5480,7 @@
         <v>14</v>
       </c>
       <c r="D64">
-        <v>1.640625</v>
+        <v>1.65625</v>
       </c>
       <c r="E64" t="s">
         <v>14</v>
@@ -5496,7 +5494,7 @@
         <v>50</v>
       </c>
       <c r="D65">
-        <v>3.53125</v>
+        <v>3.640625</v>
       </c>
       <c r="E65" t="s">
         <v>50</v>
@@ -5510,7 +5508,7 @@
         <v>77</v>
       </c>
       <c r="D66">
-        <v>3.765625</v>
+        <v>3.859375</v>
       </c>
       <c r="E66" t="s">
         <v>77</v>
@@ -5524,7 +5522,7 @@
         <v>32</v>
       </c>
       <c r="D67">
-        <v>5.484375</v>
+        <v>5.65625</v>
       </c>
       <c r="E67" t="s">
         <v>32</v>
@@ -5538,7 +5536,7 @@
         <v>54</v>
       </c>
       <c r="D68">
-        <v>4.609375</v>
+        <v>4.671875</v>
       </c>
       <c r="E68" t="s">
         <v>54</v>
@@ -5552,7 +5550,7 @@
         <v>64</v>
       </c>
       <c r="D69">
-        <v>5.46875</v>
+        <v>5.609375</v>
       </c>
       <c r="E69" t="s">
         <v>64</v>
@@ -5560,7 +5558,7 @@
     </row>
     <row r="70" spans="1:5">
       <c r="D70">
-        <v>0.34375</v>
+        <v>5.875</v>
       </c>
       <c r="E70" t="s">
         <v>90</v>
@@ -5574,7 +5572,7 @@
         <v>58</v>
       </c>
       <c r="D71">
-        <v>1.5</v>
+        <v>1.546875</v>
       </c>
       <c r="E71" t="s">
         <v>58</v>
@@ -5588,7 +5586,7 @@
         <v>67</v>
       </c>
       <c r="D72">
-        <v>6.890625</v>
+        <v>7.0625</v>
       </c>
       <c r="E72" t="s">
         <v>67</v>
@@ -5602,7 +5600,7 @@
         <v>63</v>
       </c>
       <c r="D73">
-        <v>3.84375</v>
+        <v>3.984375</v>
       </c>
       <c r="E73" t="s">
         <v>63</v>
@@ -5616,7 +5614,7 @@
         <v>48</v>
       </c>
       <c r="D74">
-        <v>4.015625</v>
+        <v>4.203125</v>
       </c>
       <c r="E74" t="s">
         <v>48</v>
@@ -5630,7 +5628,7 @@
         <v>82</v>
       </c>
       <c r="D75">
-        <v>4.921875</v>
+        <v>5.09375</v>
       </c>
       <c r="E75" t="s">
         <v>82</v>
@@ -5644,7 +5642,7 @@
         <v>30</v>
       </c>
       <c r="D76">
-        <v>5.71875</v>
+        <v>5.84375</v>
       </c>
       <c r="E76" t="s">
         <v>30</v>
@@ -5658,7 +5656,7 @@
         <v>26</v>
       </c>
       <c r="D77">
-        <v>3.96875</v>
+        <v>4.046875</v>
       </c>
       <c r="E77" t="s">
         <v>26</v>
@@ -5672,7 +5670,7 @@
         <v>40</v>
       </c>
       <c r="D78">
-        <v>4.28125</v>
+        <v>4.40625</v>
       </c>
       <c r="E78" t="s">
         <v>40</v>
@@ -5686,7 +5684,7 @@
         <v>35</v>
       </c>
       <c r="D79">
-        <v>5</v>
+        <v>5.171875</v>
       </c>
       <c r="E79" t="s">
         <v>35</v>
@@ -5700,7 +5698,7 @@
         <v>46</v>
       </c>
       <c r="D80">
-        <v>4.375</v>
+        <v>4.46875</v>
       </c>
       <c r="E80" t="s">
         <v>46</v>
@@ -5714,7 +5712,7 @@
         <v>79</v>
       </c>
       <c r="D81">
-        <v>4.296875</v>
+        <v>4.421875</v>
       </c>
       <c r="E81" t="s">
         <v>79</v>
@@ -5728,7 +5726,7 @@
         <v>47</v>
       </c>
       <c r="D82">
-        <v>5.671875</v>
+        <v>5.828125</v>
       </c>
       <c r="E82" t="s">
         <v>47</v>
@@ -5742,7 +5740,7 @@
         <v>61</v>
       </c>
       <c r="D83">
-        <v>4.328125</v>
+        <v>4.46875</v>
       </c>
       <c r="E83" t="s">
         <v>61</v>
@@ -5756,7 +5754,7 @@
         <v>68</v>
       </c>
       <c r="D84">
-        <v>4.25</v>
+        <v>4.40625</v>
       </c>
       <c r="E84" t="s">
         <v>68</v>
@@ -5770,7 +5768,7 @@
         <v>60</v>
       </c>
       <c r="D85">
-        <v>2.453125</v>
+        <v>2.578125</v>
       </c>
       <c r="E85" t="s">
         <v>60</v>
@@ -5784,7 +5782,7 @@
         <v>24</v>
       </c>
       <c r="D86">
-        <v>1.46875</v>
+        <v>1.5</v>
       </c>
       <c r="E86" t="s">
         <v>24</v>
@@ -5798,7 +5796,7 @@
         <v>57</v>
       </c>
       <c r="D87">
-        <v>1.640625</v>
+        <v>1.671875</v>
       </c>
       <c r="E87" t="s">
         <v>57</v>
@@ -5812,7 +5810,7 @@
         <v>16</v>
       </c>
       <c r="D88">
-        <v>1.640625</v>
+        <v>1.65625</v>
       </c>
       <c r="E88" t="s">
         <v>16</v>
@@ -5826,7 +5824,7 @@
         <v>51</v>
       </c>
       <c r="D89">
-        <v>5.078125</v>
+        <v>5.265625</v>
       </c>
       <c r="E89" t="s">
         <v>51</v>
@@ -5840,7 +5838,7 @@
         <v>49</v>
       </c>
       <c r="D90">
-        <v>5.03125</v>
+        <v>5.125</v>
       </c>
       <c r="E90" t="s">
         <v>49</v>
@@ -5854,7 +5852,7 @@
         <v>21</v>
       </c>
       <c r="D91">
-        <v>1.515625</v>
+        <v>1.5625</v>
       </c>
       <c r="E91" t="s">
         <v>21</v>
@@ -5868,7 +5866,7 @@
         <v>28</v>
       </c>
       <c r="D92">
-        <v>4.03125</v>
+        <v>4.140625</v>
       </c>
       <c r="E92" t="s">
         <v>28</v>
@@ -5882,7 +5880,7 @@
         <v>81</v>
       </c>
       <c r="D93">
-        <v>4.765625</v>
+        <v>4.921875</v>
       </c>
       <c r="E93" t="s">
         <v>81</v>
@@ -5896,7 +5894,7 @@
         <v>43</v>
       </c>
       <c r="D94">
-        <v>4.015625</v>
+        <v>4.140625</v>
       </c>
       <c r="E94" t="s">
         <v>43</v>
@@ -5904,7 +5902,7 @@
     </row>
     <row r="95" spans="1:5">
       <c r="D95">
-        <v>0.34375</v>
+        <v>0.359375</v>
       </c>
       <c r="E95" t="s">
         <v>91</v>

</xml_diff>